<commit_message>
More finetune of eval. Pending debug.
</commit_message>
<xml_diff>
--- a/SquareWeight.xlsx
+++ b/SquareWeight.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25200" windowHeight="12090"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -54,25 +54,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -92,18 +78,48 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,13 +139,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -138,14 +147,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -159,25 +176,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,7 +185,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,192 +206,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -400,11 +400,132 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -426,11 +547,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -440,30 +559,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,172 +577,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -658,6 +738,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,15 +1086,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:J55"/>
+  <dimension ref="A3:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,8 +1123,23 @@
         <f>F3</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="M3" s="4">
+        <v>15</v>
+      </c>
+      <c r="N3" s="5">
+        <v>75</v>
+      </c>
+      <c r="O3" s="5">
+        <v>29</v>
+      </c>
+      <c r="P3" s="5">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1044,8 +1166,23 @@
         <f t="shared" ref="J4:J12" si="1">F4</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="M4" s="6">
+        <v>28</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>35</v>
+      </c>
+      <c r="P4">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1072,8 +1209,23 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="M5" s="6">
+        <v>52</v>
+      </c>
+      <c r="N5">
+        <v>31</v>
+      </c>
+      <c r="O5">
+        <v>101</v>
+      </c>
+      <c r="P5">
+        <v>64</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1100,8 +1252,23 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="M6" s="6">
+        <v>39</v>
+      </c>
+      <c r="N6">
+        <v>64</v>
+      </c>
+      <c r="O6">
+        <v>66</v>
+      </c>
+      <c r="P6">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="1:17">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1127,6 +1294,21 @@
       <c r="J7">
         <f t="shared" si="1"/>
         <v>4</v>
+      </c>
+      <c r="M7" s="7">
+        <v>55</v>
+      </c>
+      <c r="N7" s="8">
+        <v>71</v>
+      </c>
+      <c r="O7" s="8">
+        <v>129</v>
+      </c>
+      <c r="P7" s="8">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1241,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:21">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1268,23 +1450,131 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="M12" s="9">
+        <v>3</v>
+      </c>
+      <c r="N12" s="9">
+        <v>52</v>
+      </c>
+      <c r="O12" s="9">
+        <v>24</v>
+      </c>
+      <c r="P12" s="9">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>1</v>
+      </c>
+      <c r="R12" s="9">
+        <v>25</v>
+      </c>
+      <c r="S12" s="9">
+        <v>27</v>
+      </c>
+      <c r="T12" s="9">
+        <v>59</v>
+      </c>
+      <c r="U12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="M13" s="9">
+        <v>2</v>
+      </c>
+      <c r="N13" s="9">
+        <v>3</v>
+      </c>
+      <c r="O13" s="9">
+        <v>5</v>
+      </c>
+      <c r="P13" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>22</v>
+      </c>
+      <c r="R13" s="9">
+        <v>3</v>
+      </c>
+      <c r="S13" s="9">
+        <v>8</v>
+      </c>
+      <c r="T13" s="9">
+        <v>4</v>
+      </c>
+      <c r="U13" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="M14" s="9">
+        <v>14</v>
+      </c>
+      <c r="N14" s="9">
+        <v>15</v>
+      </c>
+      <c r="O14" s="9">
+        <v>34</v>
+      </c>
+      <c r="P14" s="9">
+        <v>37</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>69</v>
+      </c>
+      <c r="R14" s="9">
+        <v>29</v>
+      </c>
+      <c r="S14" s="9">
+        <v>34</v>
+      </c>
+      <c r="T14" s="9">
+        <v>7</v>
+      </c>
+      <c r="U14" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="M15" s="9">
+        <v>79</v>
+      </c>
+      <c r="N15" s="9">
+        <v>6</v>
+      </c>
+      <c r="O15" s="9">
+        <v>89</v>
+      </c>
+      <c r="P15" s="9">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>181</v>
+      </c>
+      <c r="R15" s="9">
+        <v>19</v>
+      </c>
+      <c r="S15" s="9">
+        <v>55</v>
+      </c>
+      <c r="T15" s="9">
+        <v>4</v>
+      </c>
+      <c r="U15" s="9">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1310,8 +1600,35 @@
         <f>H2+I3+G3</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="M16" s="9">
+        <v>31</v>
+      </c>
+      <c r="N16" s="9">
+        <v>14</v>
+      </c>
+      <c r="O16" s="9">
+        <v>88</v>
+      </c>
+      <c r="P16" s="9">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>66</v>
+      </c>
+      <c r="R16" s="9">
+        <v>26</v>
+      </c>
+      <c r="S16" s="9">
+        <v>75</v>
+      </c>
+      <c r="T16" s="9">
+        <v>13</v>
+      </c>
+      <c r="U16" s="9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1335,8 +1652,35 @@
         <f>H3+I4+G4</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="M17" s="9">
+        <v>36</v>
+      </c>
+      <c r="N17" s="9">
+        <v>21</v>
+      </c>
+      <c r="O17" s="9">
+        <v>75</v>
+      </c>
+      <c r="P17" s="9">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>36</v>
+      </c>
+      <c r="R17" s="9">
+        <v>30</v>
+      </c>
+      <c r="S17" s="9">
+        <v>100</v>
+      </c>
+      <c r="T17" s="9">
+        <v>16</v>
+      </c>
+      <c r="U17" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1360,8 +1704,35 @@
         <f>H4+I5+G5</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="M18" s="9">
+        <v>8</v>
+      </c>
+      <c r="N18" s="9">
+        <v>9</v>
+      </c>
+      <c r="O18" s="9">
+        <v>17</v>
+      </c>
+      <c r="P18" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>43</v>
+      </c>
+      <c r="R18" s="9">
+        <v>7</v>
+      </c>
+      <c r="S18" s="9">
+        <v>16</v>
+      </c>
+      <c r="T18" s="9">
+        <v>13</v>
+      </c>
+      <c r="U18" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1385,8 +1756,35 @@
         <f>H5+I6+G6</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="M19" s="9">
+        <v>11</v>
+      </c>
+      <c r="N19" s="9">
+        <v>4</v>
+      </c>
+      <c r="O19" s="9">
+        <v>16</v>
+      </c>
+      <c r="P19" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>31</v>
+      </c>
+      <c r="R19" s="9">
+        <v>14</v>
+      </c>
+      <c r="S19" s="9">
+        <v>14</v>
+      </c>
+      <c r="T19" s="9">
+        <v>8</v>
+      </c>
+      <c r="U19" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1410,8 +1808,35 @@
         <f>H6+I7+G7</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="M20" s="9">
+        <v>1</v>
+      </c>
+      <c r="N20" s="9">
+        <v>1</v>
+      </c>
+      <c r="O20" s="9">
+        <v>4</v>
+      </c>
+      <c r="P20" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>11</v>
+      </c>
+      <c r="R20" s="9">
+        <v>6</v>
+      </c>
+      <c r="S20" s="9">
+        <v>4</v>
+      </c>
+      <c r="T20" s="9">
+        <v>14</v>
+      </c>
+      <c r="U20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1427,8 +1852,35 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="M21" s="9">
+        <v>1</v>
+      </c>
+      <c r="N21" s="9">
+        <v>34</v>
+      </c>
+      <c r="O21" s="9">
+        <v>5</v>
+      </c>
+      <c r="P21" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>2</v>
+      </c>
+      <c r="R21" s="9">
+        <v>6</v>
+      </c>
+      <c r="S21" s="9">
+        <v>3</v>
+      </c>
+      <c r="T21" s="9">
+        <v>22</v>
+      </c>
+      <c r="U21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1444,23 +1896,113 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="M23" s="9">
+        <v>3</v>
+      </c>
+      <c r="N23" s="9">
+        <v>49</v>
+      </c>
+      <c r="O23" s="9">
+        <v>5</v>
+      </c>
+      <c r="P23" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>1</v>
+      </c>
+      <c r="R23" s="9">
+        <v>7</v>
+      </c>
+      <c r="S23" s="9">
+        <v>8</v>
+      </c>
+      <c r="T23" s="9">
+        <v>52</v>
+      </c>
+      <c r="U23" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="M24" s="9">
+        <v>2</v>
+      </c>
+      <c r="N24" s="9">
+        <v>3</v>
+      </c>
+      <c r="O24" s="9">
+        <v>9</v>
+      </c>
+      <c r="P24" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>10</v>
+      </c>
+      <c r="R24" s="9">
+        <v>4</v>
+      </c>
+      <c r="S24" s="9">
+        <v>6</v>
+      </c>
+      <c r="T24" s="9">
+        <v>2</v>
+      </c>
+      <c r="U24" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="M25" s="9">
+        <v>8</v>
+      </c>
+      <c r="N25" s="9">
+        <v>14</v>
+      </c>
+      <c r="O25" s="9">
+        <v>16</v>
+      </c>
+      <c r="P25" s="9">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>28</v>
+      </c>
+      <c r="R25" s="9">
+        <v>12</v>
+      </c>
+      <c r="S25" s="9">
+        <v>14</v>
+      </c>
+      <c r="T25" s="9">
+        <v>4</v>
+      </c>
+      <c r="U25" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1486,8 +2028,35 @@
         <f t="shared" ref="H26:H35" si="8">(F4+G5+I5+J4+J2+I1+G1+F2)/2</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="M26" s="9">
+        <v>9</v>
+      </c>
+      <c r="N26" s="9">
+        <v>9</v>
+      </c>
+      <c r="O26" s="9">
+        <v>24</v>
+      </c>
+      <c r="P26" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>66</v>
+      </c>
+      <c r="R26" s="9">
+        <v>20</v>
+      </c>
+      <c r="S26" s="9">
+        <v>9</v>
+      </c>
+      <c r="T26" s="9">
+        <v>4</v>
+      </c>
+      <c r="U26" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1511,8 +2080,35 @@
         <f t="shared" si="8"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="M27" s="9">
+        <v>11</v>
+      </c>
+      <c r="N27" s="9">
+        <v>13</v>
+      </c>
+      <c r="O27" s="9">
+        <v>82</v>
+      </c>
+      <c r="P27" s="9">
+        <v>25</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>56</v>
+      </c>
+      <c r="R27" s="9">
+        <v>18</v>
+      </c>
+      <c r="S27" s="9">
+        <v>77</v>
+      </c>
+      <c r="T27" s="9">
+        <v>12</v>
+      </c>
+      <c r="U27" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1536,8 +2132,35 @@
         <f t="shared" si="8"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="M28" s="9">
+        <v>50</v>
+      </c>
+      <c r="N28" s="9">
+        <v>18</v>
+      </c>
+      <c r="O28" s="9">
+        <v>106</v>
+      </c>
+      <c r="P28" s="9">
+        <v>21</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>50</v>
+      </c>
+      <c r="R28" s="9">
+        <v>31</v>
+      </c>
+      <c r="S28" s="9">
+        <v>113</v>
+      </c>
+      <c r="T28" s="9">
+        <v>14</v>
+      </c>
+      <c r="U28" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1561,8 +2184,35 @@
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="M29" s="9">
+        <v>91</v>
+      </c>
+      <c r="N29" s="9">
+        <v>9</v>
+      </c>
+      <c r="O29" s="9">
+        <v>47</v>
+      </c>
+      <c r="P29" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>116</v>
+      </c>
+      <c r="R29" s="9">
+        <v>6</v>
+      </c>
+      <c r="S29" s="9">
+        <v>76</v>
+      </c>
+      <c r="T29" s="9">
+        <v>8</v>
+      </c>
+      <c r="U29" s="9">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1586,8 +2236,35 @@
         <f t="shared" si="8"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="M30" s="9">
+        <v>25</v>
+      </c>
+      <c r="N30" s="9">
+        <v>10</v>
+      </c>
+      <c r="O30" s="9">
+        <v>25</v>
+      </c>
+      <c r="P30" s="9">
+        <v>24</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>59</v>
+      </c>
+      <c r="R30" s="9">
+        <v>41</v>
+      </c>
+      <c r="S30" s="9">
+        <v>36</v>
+      </c>
+      <c r="T30" s="9">
+        <v>10</v>
+      </c>
+      <c r="U30" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1611,8 +2288,35 @@
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="M31" s="9">
+        <v>4</v>
+      </c>
+      <c r="N31" s="9">
+        <v>2</v>
+      </c>
+      <c r="O31" s="9">
+        <v>3</v>
+      </c>
+      <c r="P31" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>22</v>
+      </c>
+      <c r="R31" s="9">
+        <v>5</v>
+      </c>
+      <c r="S31" s="9">
+        <v>4</v>
+      </c>
+      <c r="T31" s="9">
+        <v>9</v>
+      </c>
+      <c r="U31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1635,6 +2339,33 @@
       <c r="H32" s="3">
         <f t="shared" si="8"/>
         <v>16</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0</v>
+      </c>
+      <c r="N32" s="9">
+        <v>32</v>
+      </c>
+      <c r="O32" s="9">
+        <v>24</v>
+      </c>
+      <c r="P32" s="9">
+        <v>23</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>2</v>
+      </c>
+      <c r="R32" s="9">
+        <v>20</v>
+      </c>
+      <c r="S32" s="9">
+        <v>27</v>
+      </c>
+      <c r="T32" s="9">
+        <v>23</v>
+      </c>
+      <c r="U32" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1879,6 +2610,30 @@
     <mergeCell ref="A36:A45"/>
     <mergeCell ref="A46:A55"/>
   </mergeCells>
+  <conditionalFormatting sqref="M12:U21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M23:U32">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>